<commit_message>
building codes updated, alternative calculation of transmission
</commit_message>
<xml_diff>
--- a/resources/parameters/Waermebedarfskennwerte (IWU).xlsx
+++ b/resources/parameters/Waermebedarfskennwerte (IWU).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\PycharmProjects\PBE1\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\PycharmProjects\pbe1\resources\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739A9EAC-5F47-4CCE-A9EC-E0EFA69E2537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F949C73C-5B57-4D01-A503-FC95B15981A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="142">
   <si>
     <t>Gebäudetyp</t>
   </si>
@@ -523,6 +523,18 @@
   </si>
   <si>
     <t>Apartments</t>
+  </si>
+  <si>
+    <t>RH_F</t>
+  </si>
+  <si>
+    <t>RH_J</t>
+  </si>
+  <si>
+    <t>RH_E</t>
+  </si>
+  <si>
+    <t>HH_E</t>
   </si>
 </sst>
 </file>
@@ -1960,8 +1972,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83EAF153-A14F-4496-918A-BEEA1A456304}" name="Tabelle1" displayName="Tabelle1" ref="A1:H9" totalsRowShown="0">
-  <autoFilter ref="A1:H9" xr:uid="{83EAF153-A14F-4496-918A-BEEA1A456304}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83EAF153-A14F-4496-918A-BEEA1A456304}" name="Tabelle1" displayName="Tabelle1" ref="A1:H13" totalsRowShown="0">
+  <autoFilter ref="A1:H13" xr:uid="{83EAF153-A14F-4496-918A-BEEA1A456304}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A8B03A52-44E8-4AA4-B782-9E854BE728C0}" name="Code"/>
     <tableColumn id="2" xr3:uid="{A13DE8AE-6C3B-456A-A744-89C65B6B6022}" name="Typ"/>
@@ -7467,10 +7479,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393DAACF-8588-40C1-B092-870998C37784}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7689,12 +7701,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C9">
         <v>1958</v>
@@ -7703,15 +7712,110 @@
         <v>1968</v>
       </c>
       <c r="E9">
+        <v>1.05</v>
+      </c>
+      <c r="F9">
+        <v>1.46</v>
+      </c>
+      <c r="G9">
+        <v>143.6</v>
+      </c>
+      <c r="H9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10">
+        <v>1969</v>
+      </c>
+      <c r="D10">
+        <v>1978</v>
+      </c>
+      <c r="E10">
+        <v>0.99</v>
+      </c>
+      <c r="F10">
+        <v>2.06</v>
+      </c>
+      <c r="G10">
+        <v>177.7</v>
+      </c>
+      <c r="H10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11">
+        <v>2002</v>
+      </c>
+      <c r="D11">
+        <v>2009</v>
+      </c>
+      <c r="E11">
+        <v>0.41</v>
+      </c>
+      <c r="F11" s="39">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>83.1</v>
+      </c>
+      <c r="H11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12">
+        <v>1958</v>
+      </c>
+      <c r="D12">
+        <v>1968</v>
+      </c>
+      <c r="E12">
+        <v>1.57</v>
+      </c>
+      <c r="F12">
+        <v>1.53</v>
+      </c>
+      <c r="G12">
+        <v>130.1</v>
+      </c>
+      <c r="H12">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13">
+        <v>1958</v>
+      </c>
+      <c r="D13">
+        <v>1968</v>
+      </c>
+      <c r="E13">
         <v>1.42</v>
       </c>
-      <c r="F9">
+      <c r="F13">
         <v>1.96</v>
       </c>
-      <c r="G9">
+      <c r="G13">
         <v>161.4</v>
       </c>
-      <c r="H9">
+      <c r="H13">
         <v>52.5</v>
       </c>
     </row>

</xml_diff>